<commit_message>
done crud siswa and import by excel
</commit_message>
<xml_diff>
--- a/ml/data_test/data_10baris.xlsx
+++ b/ml/data_test/data_10baris.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TRIO\Dicoding\Coding Camp 2025\Capstone\capstone_spk_pip\ml\data_test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodingCamp DBS\Capstone\capstone_spk_pip\ml\data_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C6D2BA-150D-49D5-9C6C-93BCE0BD9702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C62C8BD-20C4-47B0-BBBD-ABD482545711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="28">
   <si>
     <t>Alat Transportasi</t>
   </si>
@@ -71,6 +71,39 @@
   </si>
   <si>
     <t>Ya</t>
+  </si>
+  <si>
+    <t>Nama Siswa</t>
+  </si>
+  <si>
+    <t>Ucup</t>
+  </si>
+  <si>
+    <t>Ujank</t>
+  </si>
+  <si>
+    <t>Umar</t>
+  </si>
+  <si>
+    <t>Khabib</t>
+  </si>
+  <si>
+    <t>Fadil</t>
+  </si>
+  <si>
+    <t>Prakoso</t>
+  </si>
+  <si>
+    <t>Fariz</t>
+  </si>
+  <si>
+    <t>Trio</t>
+  </si>
+  <si>
+    <t>Azel</t>
+  </si>
+  <si>
+    <t>Dafa</t>
   </si>
 </sst>
 </file>
@@ -438,239 +471,272 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>4213001</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
       <c r="F2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>3249958</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
       <c r="F3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>4166323</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
       <c r="F4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>3261966</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
       <c r="F5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>3254943</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
       <c r="F6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>3500000</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
       </c>
       <c r="F7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>3100000</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>14</v>
       </c>
-      <c r="E8" t="s">
-        <v>15</v>
-      </c>
       <c r="F8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>3200000</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>13</v>
-      </c>
-      <c r="E9" t="s">
-        <v>16</v>
       </c>
       <c r="F9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>4000000</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>12</v>
       </c>
-      <c r="E10" t="s">
-        <v>15</v>
-      </c>
       <c r="F10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>10</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>3300000</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>14</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>16</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>